<commit_message>
New Code changed for 3 browser execution
</commit_message>
<xml_diff>
--- a/data/TestConfiguration.xlsx
+++ b/data/TestConfiguration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KYCDemo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KYCDemo\KYCDemo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Description</t>
   </si>
@@ -80,22 +80,31 @@
     <t>120</t>
   </si>
   <si>
+    <t>version type</t>
+  </si>
+  <si>
+    <t>Application URL-DUP</t>
+  </si>
+  <si>
+    <t>https://global-stg.transak.com/</t>
+  </si>
+  <si>
+    <t>KYC</t>
+  </si>
+  <si>
+    <t>ParallelTests</t>
+  </si>
+  <si>
+    <t>Execution env</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Sequential</t>
+  </si>
+  <si>
     <t>Chrome</t>
-  </si>
-  <si>
-    <t>Sequential</t>
-  </si>
-  <si>
-    <t>version type</t>
-  </si>
-  <si>
-    <t>Application URL-DUP</t>
-  </si>
-  <si>
-    <t>https://global-stg.transak.com/</t>
-  </si>
-  <si>
-    <t>KYC</t>
   </si>
 </sst>
 </file>
@@ -495,7 +504,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <tableColumns count="3">
     <tableColumn id="1" name="Description" dataDxfId="2"/>
     <tableColumn id="2" name="Components" dataDxfId="1"/>
@@ -792,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +834,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -836,77 +845,93 @@
         <v>6</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A4" s="6"/>
       <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A5" s="6"/>
       <c r="B5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>12</v>
+      <c r="A6" s="6"/>
+      <c r="B6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>22</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
       <formula1>"Sequential,Parallel"</formula1>
       <formula2>0</formula2>
@@ -915,12 +940,18 @@
       <formula1>"Chrome,Firefox,IE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C11">
       <formula1>"https://www.nexaexperience.com/maruti-suzuki-car-finance,https://www.marutisuzuki.com/more-from-us/finance"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+      <formula1>"1,2,3,4,5,6,7,8"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
+      <formula1>"Local, Remote"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>